<commit_message>
Removed Upload data button from home menu, button was replaced with a drop&drag in the add data page . minor design changes.
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>test</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>ohiadv</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D788D7CC-192B-4F5D-85B5-B142119D78B6}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -625,6 +628,29 @@
         <v>26</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Drag Functionality To the whole graphical user interface, major graphical change + Treatment.java is modified and working
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97252\Desktop\Medical-Diagnosis\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="8">
   <si>
     <t>firstname</t>
   </si>
@@ -56,12 +56,16 @@
   </si>
   <si>
     <t>fadybd1@gmail.com</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D788D7CC-192B-4F5D-85B5-B142119D78B6}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
@@ -428,7 +432,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -481,6 +485,84 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple treatment choices are added, all question answers are now stored in seperate sets and the blood test values are in hashtables.
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>sdfsddasg</t>
+  </si>
+  <si>
+    <t>iamnumber10</t>
+  </si>
+  <si>
+    <t>hamode</t>
+  </si>
+  <si>
+    <t>hamode@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -463,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D788D7CC-192B-4F5D-85B5-B142119D78B6}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -578,6 +587,26 @@
         <v>1.23456789E9</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2.9208154E7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5.48177167E8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{6B61DFF4-B3CD-4DA8-B084-DC939BBF8C16}"/>

</xml_diff>